<commit_message>
dated on 21 feb 2020,specially for responsecode resourse
</commit_message>
<xml_diff>
--- a/Data/testdata.xlsx
+++ b/Data/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Read" sheetId="1" state="visible" r:id="rId2"/>
@@ -410,7 +410,7 @@
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">Event On Feb First</t>
+    <t xml:space="preserve">2020-2021 for Sanity</t>
   </si>
 </sst>
 </file>
@@ -620,7 +620,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -713,15 +713,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -812,8 +808,8 @@
   </sheetPr>
   <dimension ref="A1:BD51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -822,7 +818,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.65"/>
@@ -1394,7 +1390,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1465,7 +1461,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://mckcms.e2m.live/"/>
     <hyperlink ref="B4" r:id="rId2" display="https://thefuturesinstcms.e2m.live"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://truliantcms"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://truliantcms.e2m.live"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1510,7 +1506,7 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -1597,12 +1593,12 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="25" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1620,24 +1616,21 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="26" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J16" s="25" t="s">
+      <c r="J16" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J19" s="27" t="s">
+      <c r="J19" s="26" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" display="Event On Feb First"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
new code on 10th march 2020
</commit_message>
<xml_diff>
--- a/Data/testdata.xlsx
+++ b/Data/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Read" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="Varification" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Execution" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Event" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="EventSetup" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="165">
   <si>
     <t xml:space="preserve">TC_ID [0,0]</t>
   </si>
@@ -353,6 +354,12 @@
     <t xml:space="preserve">Headless</t>
   </si>
   <si>
+    <t xml:space="preserve">Pcoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pcoacms.e2m.live/ </t>
+  </si>
+  <si>
     <t xml:space="preserve">Event_Name</t>
   </si>
   <si>
@@ -411,6 +418,135 @@
   </si>
   <si>
     <t xml:space="preserve">2020-2021 for Sanity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venue_Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disclaimer_Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acceptance_Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UseFul_Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UseFul_Tag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected_useful_Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sociallink_Url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TopBar_Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Header_Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Font_Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sidenavigation_Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iPhomeImage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BackGroundType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Images Gallery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EventUsesBackground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karunamayee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARMY1112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DressCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://instagram.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBackgroundImages\backgroundImages\import1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upload Images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBackgroundImages\backgroundImages\import2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBackgroundImages\backgroundImages\import3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBackgroundImages\backgroundImages\import4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBanner\Banner\iPhone5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBanner\Banner\iPhone6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBanner\Banner\iPhone6+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBanner\Banner\iPhone10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBanner\Banner\AllAndroidPhone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBanner\Banner\iPadPortrait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBanner\Banner\iPadlandscape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.53.1</t>
   </si>
 </sst>
 </file>
@@ -421,7 +557,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -541,6 +677,13 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -620,7 +763,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -726,6 +869,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -808,7 +959,7 @@
   </sheetPr>
   <dimension ref="A1:BD51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
@@ -1388,10 +1539,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1457,11 +1608,20 @@
         <v>99</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://mckcms.e2m.live/"/>
     <hyperlink ref="B4" r:id="rId2" display="https://thefuturesinstcms.e2m.live"/>
     <hyperlink ref="B5" r:id="rId3" display="https://truliantcms.e2m.live"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://pcoacms.e2m.live/ "/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1506,7 +1666,7 @@
   </sheetPr>
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -1525,66 +1685,66 @@
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1628,6 +1788,199 @@
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J19" s="26" t="s">
         <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="116.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M1" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M3" s="15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M4" s="15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M5" s="15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M6" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M7" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M8" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M9" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M10" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M11" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M12" s="15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M20" s="23" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit on 12th feb 2020
</commit_message>
<xml_diff>
--- a/Data/testdata.xlsx
+++ b/Data/testdata.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="170">
   <si>
     <t xml:space="preserve">TC_ID [0,0]</t>
   </si>
@@ -468,7 +468,13 @@
     <t xml:space="preserve">EventUsesBackground</t>
   </si>
   <si>
-    <t xml:space="preserve">s</t>
+    <t xml:space="preserve">ResourseType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResourseTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResourseLink</t>
   </si>
   <si>
     <t xml:space="preserve">Karunamayee</t>
@@ -514,6 +520,15 @@
   </si>
   <si>
     <t xml:space="preserve">Custom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Link </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily Advertisement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://toi.com</t>
   </si>
   <si>
     <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBackgroundImages\backgroundImages\import2</t>
@@ -683,6 +698,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1806,10 +1822,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1874,113 +1890,128 @@
       <c r="P1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="Q1" s="2" t="s">
         <v>138</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="N2" s="28" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="O2" s="26" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="P2" s="26" t="s">
-        <v>153</v>
+        <v>155</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M3" s="15" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M4" s="15" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M5" s="15" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M6" s="15" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M7" s="15" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M8" s="15" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M9" s="15" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M10" s="15" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M11" s="15" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M12" s="15" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M20" s="23" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code on 18th march
</commit_message>
<xml_diff>
--- a/Data/testdata.xlsx
+++ b/Data/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Read" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,8 @@
     <sheet name="Execution" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Event" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="EventSetup" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="DataCompaire" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="DataCompaire1" r:id="rId10" sheetId="8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="162">
   <si>
     <t xml:space="preserve">TC_ID [0,0]</t>
   </si>
@@ -477,58 +479,25 @@
     <t xml:space="preserve">ResourseLink</t>
   </si>
   <si>
-    <t xml:space="preserve">Karunamayee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARMY1112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DressCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instagram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://instagram.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">grey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBackgroundImages\backgroundImages\import1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upload Images</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Custom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Link </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily Advertisement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://toi.com</t>
+    <t xml:space="preserve">Menu_Responsive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exhibitors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schedule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speakers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sponsors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unpublished</t>
   </si>
   <si>
     <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBackgroundImages\backgroundImages\import2</t>
@@ -561,7 +530,16 @@
     <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\GBBranding\AppBranding\EventBanner\Banner\iPadlandscape</t>
   </si>
   <si>
+    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\Brochure_Resourse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C:\Users\pravakar.rana\Downloads\AutomationTest\Test_Video</t>
+  </si>
+  <si>
     <t xml:space="preserve">2.53.1</t>
+  </si>
+  <si>
+    <t>Published</t>
   </si>
 </sst>
 </file>
@@ -892,7 +870,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -981,20 +959,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="9.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="35.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.67"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="6.67" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="10.32" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="10.05" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="17.36" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="11.3" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="0" width="12.04" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="0" width="12.5" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="0" width="10.65" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="0" width="13.73" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="0" width="11.94" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="true" hidden="false" style="0" width="9.17" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="0" width="11.25" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="0" width="35.58" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="1025" customWidth="true" hidden="false" style="0" width="8.67" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1469,24 +1447,24 @@
   <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.08"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.67"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="11.94" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="3" customWidth="true" hidden="false" style="0" width="10.12" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="31.96" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="0" width="10.32" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="6" customWidth="true" hidden="false" style="0" width="13.24" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" customWidth="true" hidden="false" style="0" width="13.36" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="0" width="10.6" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="0" width="14.49" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="0" width="14.08" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="11" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="12" max="12" customWidth="true" hidden="false" style="0" width="15.05" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="0" width="17.92" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="1025" customWidth="true" hidden="false" style="0" width="8.67" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1563,10 +1541,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="13.63" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="30.15" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="14.35" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1662,7 +1640,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col min="1" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1688,15 +1666,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="12.27" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="2" customWidth="true" hidden="false" style="0" width="12.13" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="true" hidden="false" style="0" width="12.56" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="true" hidden="false" style="0" width="10.88" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="6" customWidth="true" hidden="false" style="0" width="11.71" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="8" customWidth="true" hidden="false" style="0" width="9.91" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="0" width="13.24" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="true" hidden="false" style="0" width="28.48" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,23 +1800,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="116.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.84"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="12.68" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="7" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="8" customWidth="true" hidden="false" style="0" width="21.82" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="0" width="13.24" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="12" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="13" max="13" customWidth="true" hidden="false" style="0" width="116.16" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="true" hidden="false" style="0" width="15.84" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1899,119 +1877,97 @@
       <c r="S1" s="2" t="s">
         <v>140</v>
       </c>
+      <c r="T1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U1" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="V1" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="W1" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="X1" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="Y1" s="19" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" s="15" t="s">
+      <c r="Y2" s="0" t="s">
         <v>147</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="N2" s="28" t="s">
-        <v>153</v>
-      </c>
-      <c r="O2" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="P2" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q2" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M3" s="15" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M4" s="15" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M5" s="15" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M6" s="15" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M7" s="15" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M8" s="15" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M9" s="15" t="s">
-        <v>165</v>
+        <v>154</v>
+      </c>
+      <c r="U9" s="28" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M10" s="15" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M11" s="15" t="s">
-        <v>167</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="U11" s="23"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M12" s="15" t="s">
-        <v>168</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M13" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M14" s="15" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M20" s="23" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2023,4 +1979,66 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>